<commit_message>
Cambio recursos, guion 07_06
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion06/Escaleta CN_07_06_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion06/Escaleta CN_07_06_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="255">
   <si>
     <t>Asignatura</t>
   </si>
@@ -436,12 +436,6 @@
     <t>Interactivo en el que se muestran y describen las capas esféricas de la Tierra, sus orígenes, formación  y movimientos</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Las capas esféricas de la tierra</t>
-  </si>
-  <si>
-    <t>Actividad que consolida conocimientos sobre Las capas esféricas de la tierra</t>
-  </si>
-  <si>
     <t xml:space="preserve">La geósfera y sus capas        </t>
   </si>
   <si>
@@ -466,15 +460,6 @@
     <t>Interactivo que describe y explica la composición y el funcionamiento de las capas que componen la geosfera</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: La geósfera y sus capas        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad que consolida conocimientos sobre La geósfera y sus capas        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad en la que se posicionan etiquetas, de manera ordenada, basada en una imagen de las capas que componen la geosfera </t>
-  </si>
-  <si>
     <t>Recurso M9B-01</t>
   </si>
   <si>
@@ -517,9 +502,6 @@
     <t>¿Por qué los volcanes están ubicados en lugares específicos del planeta?</t>
   </si>
   <si>
-    <t>Investigación en la que se utilizan mapas para contestar a la pregunta: ¿por qué los volcanes están ubicados en lugares específicos del planeta?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Refuerza tu aprendizaje: Los movimientos de las placas tectónicas </t>
   </si>
   <si>
@@ -556,9 +538,6 @@
     <t xml:space="preserve">Los cinco continentes </t>
   </si>
   <si>
-    <t xml:space="preserve">La deriva continental        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Interactivo en el que se muestran, describen y explican los eventos más importantes de la deriva continental     </t>
   </si>
   <si>
@@ -784,7 +763,31 @@
     <t>Actividad en la que se identifican algunas ciudades de Colombia con riesgo de sufrir movimientos sísmicos</t>
   </si>
   <si>
-    <t>Competencias; Las Corrientes de convección</t>
+    <t>Refuerza tu aprendizaje: Las capas esféricas de la Tierra</t>
+  </si>
+  <si>
+    <t>Actividad que consolida conocimientos sobre Las capas esféricas de la Tierra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La geosfera y sus capas        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad en la que se posicionan etiquetas, de manera ordenada, basadas en una imagen de las capas que componen la geosfera </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: La geosfera y sus capas        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que consolida conocimientos sobre La geosfera y sus capas        </t>
+  </si>
+  <si>
+    <t>Actividad en la que se utilizan mapas para contestar a la pregunta: ¿por qué los volcanes están ubicados en lugares específicos del planeta?</t>
+  </si>
+  <si>
+    <t>Competencias; Las corrientes de convección</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La deriva continental y sus eventos más importantes </t>
   </si>
 </sst>
 </file>
@@ -3456,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3498,13 +3501,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="99" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E1" s="99" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F1" s="99" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G1" s="99" t="s">
         <v>3</v>
@@ -3519,32 +3522,32 @@
         <v>4</v>
       </c>
       <c r="K1" s="99" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L1" s="99" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="M1" s="99" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="N1" s="99"/>
       <c r="O1" s="99" t="s">
         <v>104</v>
       </c>
       <c r="P1" s="99" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="Q1" s="99" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="R1" s="99" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="S1" s="99" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="T1" s="99" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="U1" s="99" t="s">
         <v>85</v>
@@ -3625,7 +3628,7 @@
         <v>114</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="60"/>
@@ -3661,7 +3664,7 @@
       </c>
       <c r="F5" s="49"/>
       <c r="G5" s="50" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H5" s="61">
         <v>1</v>
@@ -3670,17 +3673,17 @@
         <v>18</v>
       </c>
       <c r="J5" s="52" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="K5" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M5" s="76"/>
       <c r="N5" s="76" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="O5" s="49"/>
       <c r="P5" s="51" t="s">
@@ -3693,13 +3696,13 @@
         <v>118</v>
       </c>
       <c r="S5" s="53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T5" s="55" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="U5" s="53" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3732,16 +3735,16 @@
         <v>117</v>
       </c>
       <c r="K6" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L6" s="58" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M6" s="76" t="s">
         <v>84</v>
       </c>
       <c r="N6" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O6" s="22"/>
       <c r="P6" s="44" t="s">
@@ -3793,16 +3796,16 @@
         <v>124</v>
       </c>
       <c r="K7" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M7" s="76" t="s">
         <v>82</v>
       </c>
       <c r="N7" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="29" t="s">
@@ -3845,13 +3848,13 @@
       <c r="J8" s="24"/>
       <c r="K8" s="69"/>
       <c r="L8" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M8" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N8" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O8" s="22"/>
       <c r="P8" s="28"/>
@@ -3888,19 +3891,19 @@
         <v>19</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="K9" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M9" s="76" t="s">
         <v>99</v>
       </c>
       <c r="N9" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O9" s="22"/>
       <c r="P9" s="28" t="s">
@@ -3916,7 +3919,7 @@
         <v>119</v>
       </c>
       <c r="T9" s="27" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="U9" s="25" t="s">
         <v>121</v>
@@ -3952,16 +3955,16 @@
         <v>131</v>
       </c>
       <c r="K10" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M10" s="76" t="s">
         <v>93</v>
       </c>
       <c r="N10" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O10" s="22"/>
       <c r="P10" s="28" t="s">
@@ -4006,13 +4009,13 @@
       <c r="J11" s="24"/>
       <c r="K11" s="69"/>
       <c r="L11" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M11" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N11" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O11" s="22"/>
       <c r="P11" s="28"/>
@@ -4052,16 +4055,16 @@
         <v>136</v>
       </c>
       <c r="K12" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M12" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N12" s="76" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="O12" s="22"/>
       <c r="P12" s="28" t="s">
@@ -4074,13 +4077,13 @@
         <v>118</v>
       </c>
       <c r="S12" s="53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T12" s="27" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="U12" s="53" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4101,7 +4104,7 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="H13" s="93">
         <v>7</v>
@@ -4110,19 +4113,19 @@
         <v>19</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>138</v>
+        <v>247</v>
       </c>
       <c r="K13" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M13" s="76" t="s">
         <v>82</v>
       </c>
       <c r="N13" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="28" t="s">
@@ -4138,7 +4141,7 @@
         <v>119</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>121</v>
@@ -4155,7 +4158,7 @@
         <v>113</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="22"/>
@@ -4165,13 +4168,13 @@
       <c r="J14" s="24"/>
       <c r="K14" s="69"/>
       <c r="L14" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M14" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N14" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O14" s="22"/>
       <c r="P14" s="28"/>
@@ -4192,14 +4195,14 @@
         <v>113</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H15" s="60">
         <v>8</v>
@@ -4208,19 +4211,19 @@
         <v>19</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M15" s="76" t="s">
         <v>84</v>
       </c>
       <c r="N15" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O15" s="22"/>
       <c r="P15" s="44" t="s">
@@ -4236,7 +4239,7 @@
         <v>119</v>
       </c>
       <c r="T15" s="27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U15" s="25" t="s">
         <v>121</v>
@@ -4253,10 +4256,10 @@
         <v>113</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="23"/>
@@ -4265,13 +4268,13 @@
       <c r="J16" s="24"/>
       <c r="K16" s="69"/>
       <c r="L16" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M16" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N16" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O16" s="22"/>
       <c r="P16" s="28"/>
@@ -4292,14 +4295,14 @@
         <v>113</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="23" t="s">
-        <v>139</v>
+        <v>248</v>
       </c>
       <c r="H17" s="60">
         <v>9</v>
@@ -4308,19 +4311,19 @@
         <v>18</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K17" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L17" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M17" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N17" s="76" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="O17" s="22"/>
       <c r="P17" s="28" t="s">
@@ -4333,13 +4336,13 @@
         <v>118</v>
       </c>
       <c r="S17" s="53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T17" s="27" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="U17" s="53" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -4353,14 +4356,14 @@
         <v>113</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="23" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="H18" s="60">
         <v>10</v>
@@ -4369,19 +4372,19 @@
         <v>19</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>149</v>
+        <v>249</v>
       </c>
       <c r="K18" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L18" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M18" s="76" t="s">
         <v>69</v>
       </c>
       <c r="N18" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O18" s="22"/>
       <c r="P18" s="28" t="s">
@@ -4397,7 +4400,7 @@
         <v>119</v>
       </c>
       <c r="T18" s="27" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="U18" s="25" t="s">
         <v>121</v>
@@ -4414,14 +4417,14 @@
         <v>113</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>122</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
-        <v>147</v>
+        <v>250</v>
       </c>
       <c r="H19" s="93">
         <v>11</v>
@@ -4430,19 +4433,19 @@
         <v>19</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>148</v>
+        <v>251</v>
       </c>
       <c r="K19" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L19" s="35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M19" s="76" t="s">
         <v>82</v>
       </c>
       <c r="N19" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O19" s="7"/>
       <c r="P19" s="28" t="s">
@@ -4458,7 +4461,7 @@
         <v>119</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>121</v>
@@ -4475,7 +4478,7 @@
         <v>113</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="22"/>
@@ -4485,13 +4488,13 @@
       <c r="J20" s="24"/>
       <c r="K20" s="69"/>
       <c r="L20" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M20" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N20" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O20" s="22"/>
       <c r="P20" s="28"/>
@@ -4512,14 +4515,14 @@
         <v>113</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="23" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H21" s="60">
         <v>12</v>
@@ -4528,19 +4531,19 @@
         <v>18</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="K21" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L21" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M21" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N21" s="76" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="O21" s="22"/>
       <c r="P21" s="28" t="s">
@@ -4553,13 +4556,13 @@
         <v>118</v>
       </c>
       <c r="S21" s="53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T21" s="27" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="U21" s="53" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -4573,13 +4576,13 @@
         <v>113</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G22" s="23"/>
       <c r="H22" s="60"/>
@@ -4587,13 +4590,13 @@
       <c r="J22" s="24"/>
       <c r="K22" s="69"/>
       <c r="L22" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M22" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N22" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O22" s="22"/>
       <c r="P22" s="28"/>
@@ -4614,10 +4617,10 @@
         <v>113</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
@@ -4626,13 +4629,13 @@
       <c r="J23" s="24"/>
       <c r="K23" s="69"/>
       <c r="L23" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M23" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N23" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O23" s="22"/>
       <c r="P23" s="28"/>
@@ -4653,16 +4656,16 @@
         <v>113</v>
       </c>
       <c r="D24" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>156</v>
-      </c>
       <c r="G24" s="23" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H24" s="60">
         <v>13</v>
@@ -4671,19 +4674,19 @@
         <v>19</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="K24" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M24" s="76" t="s">
         <v>100</v>
       </c>
       <c r="N24" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O24" s="22"/>
       <c r="P24" s="28" t="s">
@@ -4699,7 +4702,7 @@
         <v>119</v>
       </c>
       <c r="T24" s="27" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="U24" s="25" t="s">
         <v>121</v>
@@ -4716,16 +4719,16 @@
         <v>113</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E25" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" s="23" t="s">
         <v>155</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>160</v>
       </c>
       <c r="H25" s="60">
         <v>14</v>
@@ -4734,19 +4737,19 @@
         <v>19</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K25" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L25" s="35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M25" s="76" t="s">
         <v>84</v>
       </c>
       <c r="N25" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O25" s="22"/>
       <c r="P25" s="44" t="s">
@@ -4762,7 +4765,7 @@
         <v>119</v>
       </c>
       <c r="T25" s="27" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>121</v>
@@ -4779,16 +4782,16 @@
         <v>113</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H26" s="60">
         <v>15</v>
@@ -4797,19 +4800,19 @@
         <v>19</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>164</v>
+        <v>252</v>
       </c>
       <c r="K26" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L26" s="35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M26" s="76" t="s">
         <v>84</v>
       </c>
       <c r="N26" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O26" s="22"/>
       <c r="P26" s="28" t="s">
@@ -4825,7 +4828,7 @@
         <v>119</v>
       </c>
       <c r="T26" s="27" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>121</v>
@@ -4842,14 +4845,14 @@
         <v>113</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>122</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H27" s="93">
         <v>16</v>
@@ -4858,19 +4861,19 @@
         <v>19</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="K27" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L27" s="39" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M27" s="76" t="s">
         <v>82</v>
       </c>
       <c r="N27" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O27" s="7"/>
       <c r="P27" s="29" t="s">
@@ -4886,7 +4889,7 @@
         <v>119</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="U27" s="10" t="s">
         <v>121</v>
@@ -4903,7 +4906,7 @@
         <v>113</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="22"/>
@@ -4913,13 +4916,13 @@
       <c r="J28" s="24"/>
       <c r="K28" s="69"/>
       <c r="L28" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M28" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N28" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O28" s="22"/>
       <c r="P28" s="28"/>
@@ -4940,10 +4943,10 @@
         <v>113</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="23"/>
@@ -4952,13 +4955,13 @@
       <c r="J29" s="24"/>
       <c r="K29" s="69"/>
       <c r="L29" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M29" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N29" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O29" s="22"/>
       <c r="P29" s="44"/>
@@ -4979,10 +4982,10 @@
         <v>113</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="23"/>
@@ -4991,13 +4994,13 @@
       <c r="J30" s="24"/>
       <c r="K30" s="69"/>
       <c r="L30" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M30" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N30" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O30" s="22"/>
       <c r="P30" s="28"/>
@@ -5018,10 +5021,10 @@
         <v>113</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="23"/>
@@ -5030,13 +5033,13 @@
       <c r="J31" s="24"/>
       <c r="K31" s="69"/>
       <c r="L31" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M31" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N31" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O31" s="22"/>
       <c r="P31" s="28"/>
@@ -5057,10 +5060,10 @@
         <v>113</v>
       </c>
       <c r="D32" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" s="19" t="s">
         <v>168</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>174</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="23"/>
@@ -5069,13 +5072,13 @@
       <c r="J32" s="24"/>
       <c r="K32" s="69"/>
       <c r="L32" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M32" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N32" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O32" s="22"/>
       <c r="P32" s="28"/>
@@ -5096,10 +5099,10 @@
         <v>113</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="23"/>
@@ -5108,13 +5111,13 @@
       <c r="J33" s="24"/>
       <c r="K33" s="69"/>
       <c r="L33" s="35" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M33" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N33" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O33" s="22"/>
       <c r="P33" s="28"/>
@@ -5135,14 +5138,14 @@
         <v>113</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="23" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H34" s="60">
         <v>17</v>
@@ -5151,19 +5154,19 @@
         <v>19</v>
       </c>
       <c r="J34" s="24" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="K34" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L34" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M34" s="76" t="s">
         <v>80</v>
       </c>
       <c r="N34" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O34" s="22"/>
       <c r="P34" s="28" t="s">
@@ -5179,7 +5182,7 @@
         <v>119</v>
       </c>
       <c r="T34" s="27" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="U34" s="25" t="s">
         <v>121</v>
@@ -5196,14 +5199,14 @@
         <v>113</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="23" t="s">
-        <v>177</v>
+        <v>254</v>
       </c>
       <c r="H35" s="60">
         <v>18</v>
@@ -5212,19 +5215,19 @@
         <v>18</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K35" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L35" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M35" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N35" s="76" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="O35" s="22"/>
       <c r="P35" s="28" t="s">
@@ -5237,13 +5240,13 @@
         <v>118</v>
       </c>
       <c r="S35" s="53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T35" s="27" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="U35" s="53" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5257,14 +5260,14 @@
         <v>113</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="23" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H36" s="60">
         <v>19</v>
@@ -5273,19 +5276,19 @@
         <v>19</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K36" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L36" s="35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M36" s="76" t="s">
         <v>68</v>
       </c>
       <c r="N36" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O36" s="22"/>
       <c r="P36" s="44" t="s">
@@ -5301,7 +5304,7 @@
         <v>119</v>
       </c>
       <c r="T36" s="27" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="U36" s="25" t="s">
         <v>121</v>
@@ -5318,14 +5321,14 @@
         <v>113</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H37" s="93">
         <v>20</v>
@@ -5334,19 +5337,19 @@
         <v>19</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K37" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L37" s="35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M37" s="76" t="s">
         <v>82</v>
       </c>
       <c r="N37" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O37" s="7"/>
       <c r="P37" s="28" t="s">
@@ -5362,7 +5365,7 @@
         <v>119</v>
       </c>
       <c r="T37" s="12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="U37" s="10" t="s">
         <v>121</v>
@@ -5379,7 +5382,7 @@
         <v>113</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E38" s="46"/>
       <c r="F38" s="49"/>
@@ -5389,13 +5392,13 @@
       <c r="J38" s="52"/>
       <c r="K38" s="70"/>
       <c r="L38" s="42" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M38" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N38" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O38" s="49"/>
       <c r="P38" s="51"/>
@@ -5416,10 +5419,10 @@
         <v>113</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F39" s="49"/>
       <c r="G39" s="50"/>
@@ -5428,13 +5431,13 @@
       <c r="J39" s="52"/>
       <c r="K39" s="70"/>
       <c r="L39" s="42" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M39" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N39" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O39" s="49"/>
       <c r="P39" s="51"/>
@@ -5455,13 +5458,13 @@
         <v>113</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F40" s="49" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G40" s="50"/>
       <c r="H40" s="61"/>
@@ -5469,13 +5472,13 @@
       <c r="J40" s="52"/>
       <c r="K40" s="70"/>
       <c r="L40" s="42" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M40" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N40" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O40" s="49"/>
       <c r="P40" s="51"/>
@@ -5496,10 +5499,10 @@
         <v>113</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E41" s="46" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F41" s="49"/>
       <c r="G41" s="50"/>
@@ -5508,13 +5511,13 @@
       <c r="J41" s="52"/>
       <c r="K41" s="70"/>
       <c r="L41" s="42" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M41" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N41" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O41" s="49"/>
       <c r="P41" s="51"/>
@@ -5535,13 +5538,13 @@
         <v>113</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E42" s="46" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F42" s="49" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G42" s="50"/>
       <c r="H42" s="61"/>
@@ -5549,13 +5552,13 @@
       <c r="J42" s="52"/>
       <c r="K42" s="70"/>
       <c r="L42" s="42" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M42" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N42" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O42" s="49"/>
       <c r="P42" s="51"/>
@@ -5576,13 +5579,13 @@
         <v>113</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E43" s="46" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F43" s="49" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G43" s="50"/>
       <c r="H43" s="61"/>
@@ -5590,13 +5593,13 @@
       <c r="J43" s="52"/>
       <c r="K43" s="70"/>
       <c r="L43" s="42" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="M43" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N43" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O43" s="49"/>
       <c r="P43" s="51"/>
@@ -5617,14 +5620,14 @@
         <v>113</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F44" s="49"/>
       <c r="G44" s="50" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H44" s="61">
         <v>21</v>
@@ -5633,19 +5636,19 @@
         <v>18</v>
       </c>
       <c r="J44" s="52" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="K44" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L44" s="42" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M44" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N44" s="76" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="O44" s="49"/>
       <c r="P44" s="51" t="s">
@@ -5658,13 +5661,13 @@
         <v>118</v>
       </c>
       <c r="S44" s="53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T44" s="55" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="U44" s="53" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5678,14 +5681,14 @@
         <v>113</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>122</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="8" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="H45" s="93">
         <v>22</v>
@@ -5694,19 +5697,19 @@
         <v>19</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="K45" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L45" s="39" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M45" s="76" t="s">
         <v>82</v>
       </c>
       <c r="N45" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O45" s="7"/>
       <c r="P45" s="29" t="s">
@@ -5722,7 +5725,7 @@
         <v>119</v>
       </c>
       <c r="T45" s="12" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="U45" s="10" t="s">
         <v>121</v>
@@ -5739,7 +5742,7 @@
         <v>113</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E46" s="46"/>
       <c r="F46" s="49"/>
@@ -5753,22 +5756,22 @@
         <v>18</v>
       </c>
       <c r="J46" s="98" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="K46" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L46" s="42" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M46" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N46" s="76" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="O46" s="49" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="P46" s="51" t="s">
         <v>18</v>
@@ -5780,13 +5783,13 @@
         <v>118</v>
       </c>
       <c r="S46" s="53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T46" s="27" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="U46" s="53" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="1:21" s="56" customFormat="1" x14ac:dyDescent="0.25">
@@ -5800,12 +5803,12 @@
         <v>113</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="49"/>
       <c r="G47" s="50" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H47" s="60">
         <v>24</v>
@@ -5814,19 +5817,19 @@
         <v>18</v>
       </c>
       <c r="J47" s="52" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="K47" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L47" s="42" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M47" s="76" t="s">
         <v>84</v>
       </c>
       <c r="N47" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O47" s="49"/>
       <c r="P47" s="51" t="s">
@@ -5842,7 +5845,7 @@
         <v>119</v>
       </c>
       <c r="T47" s="12" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="U47" s="10" t="s">
         <v>121</v>
@@ -5859,7 +5862,7 @@
         <v>113</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="49"/>
@@ -5873,19 +5876,19 @@
         <v>19</v>
       </c>
       <c r="J48" s="52" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K48" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L48" s="42" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="M48" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="N48" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O48" s="49"/>
       <c r="P48" s="51" t="s">
@@ -5908,12 +5911,12 @@
         <v>113</v>
       </c>
       <c r="D49" s="80" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E49" s="78"/>
       <c r="F49" s="81"/>
       <c r="G49" s="82" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="H49" s="94">
         <v>26</v>
@@ -5922,19 +5925,19 @@
         <v>19</v>
       </c>
       <c r="J49" s="84" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="K49" s="85" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L49" s="86" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M49" s="87" t="s">
         <v>98</v>
       </c>
       <c r="N49" s="87" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O49" s="81"/>
       <c r="P49" s="83" t="s">
@@ -5950,7 +5953,7 @@
         <v>119</v>
       </c>
       <c r="T49" s="91" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="U49" s="90" t="s">
         <v>121</v>
@@ -5967,12 +5970,12 @@
         <v>113</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="7"/>
       <c r="G50" s="8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H50" s="93">
         <v>27</v>
@@ -5981,19 +5984,19 @@
         <v>19</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="K50" s="71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L50" s="39" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M50" s="76" t="s">
         <v>83</v>
       </c>
       <c r="N50" s="76" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="O50" s="7"/>
       <c r="P50" s="68" t="s">
@@ -6252,6 +6255,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
@@ -6260,18 +6275,6 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I50">

</xml_diff>